<commit_message>
wip: changed Biofuels file format, fixed interactive accross three fist tabs
</commit_message>
<xml_diff>
--- a/data/LEAP_Biofuels.xlsx
+++ b/data/LEAP_Biofuels.xlsx
@@ -1,31 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\phoebe\GCH\Online Platform\GR_text files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ev\Documents\Software Projects\SDSN GCH\ScenViz_Template\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953200E7-4B4E-4A79-937D-73D820E7EE25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04031F28-CE75-45D1-94BE-A0D483815391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B13F852E-FF31-498A-8548-E19931A7DDEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B13F852E-FF31-498A-8548-E19931A7DDEA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Custom combinations from user" sheetId="1" r:id="rId1"/>
+    <sheet name="Production" sheetId="2" r:id="rId1"/>
+    <sheet name="Export" sheetId="3" r:id="rId2"/>
+    <sheet name="Combos" sheetId="4" r:id="rId3"/>
+    <sheet name="Custom combinations from user" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="42">
   <si>
     <t>Minimum Production Potential [ktoe]</t>
   </si>
@@ -149,6 +163,9 @@
   <si>
     <t>BLUE</t>
   </si>
+  <si>
+    <t>Code</t>
+  </si>
 </sst>
 </file>
 
@@ -157,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,7 +246,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -560,38 +577,2732 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F61CF95-A843-4AB9-8E84-263840F258FA}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2022</v>
+      </c>
+      <c r="B2">
+        <v>208.05809926435461</v>
+      </c>
+      <c r="C2">
+        <v>435.20194539982805</v>
+      </c>
+      <c r="D2">
+        <v>67.337050560490496</v>
+      </c>
+      <c r="E2">
+        <v>67.385524971336466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>222.45069743001815</v>
+      </c>
+      <c r="C3">
+        <v>454.41383395433257</v>
+      </c>
+      <c r="D3">
+        <v>67.181275041000006</v>
+      </c>
+      <c r="E3">
+        <v>66.129410714877878</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2030</v>
+      </c>
+      <c r="B4">
+        <v>229.96447167287661</v>
+      </c>
+      <c r="C4">
+        <v>466.80176865386443</v>
+      </c>
+      <c r="D4">
+        <v>66.090161846400008</v>
+      </c>
+      <c r="E4">
+        <v>51.631131049830252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2035</v>
+      </c>
+      <c r="B5">
+        <v>242.03813413585556</v>
+      </c>
+      <c r="C5">
+        <v>484.47693226330369</v>
+      </c>
+      <c r="D5">
+        <v>63.404309507500002</v>
+      </c>
+      <c r="E5">
+        <v>39.884071423753845</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2040</v>
+      </c>
+      <c r="B6">
+        <v>258.07099694277252</v>
+      </c>
+      <c r="C6">
+        <v>506.46102632081772</v>
+      </c>
+      <c r="D6">
+        <v>63.805868565400004</v>
+      </c>
+      <c r="E6">
+        <v>29.235586138563129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2045</v>
+      </c>
+      <c r="B7">
+        <v>277.44138005159067</v>
+      </c>
+      <c r="C7">
+        <v>531.89981131174159</v>
+      </c>
+      <c r="D7">
+        <v>64.285275411499995</v>
+      </c>
+      <c r="E7">
+        <v>22.084113941132991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2050</v>
+      </c>
+      <c r="B8">
+        <v>268.21928202923471</v>
+      </c>
+      <c r="C8">
+        <v>518.55353850195843</v>
+      </c>
+      <c r="D8">
+        <v>64.204841703599996</v>
+      </c>
+      <c r="E8">
+        <v>15.565188485536762</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7689DB3-4A75-4568-A4A8-BAAE0361B43E}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2022</v>
+      </c>
+      <c r="B2">
+        <v>140.72104870386411</v>
+      </c>
+      <c r="C2">
+        <v>367.86489483933758</v>
+      </c>
+      <c r="D2">
+        <v>140.67257429301816</v>
+      </c>
+      <c r="E2">
+        <v>367.8164204284916</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3">
+        <v>155.26942238901813</v>
+      </c>
+      <c r="C3">
+        <v>387.23255891333258</v>
+      </c>
+      <c r="D3">
+        <v>156.32128671514027</v>
+      </c>
+      <c r="E3">
+        <v>388.28442323945467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2030</v>
+      </c>
+      <c r="B4">
+        <v>163.8743098264766</v>
+      </c>
+      <c r="C4">
+        <v>400.71160680746442</v>
+      </c>
+      <c r="D4">
+        <v>178.33334062304635</v>
+      </c>
+      <c r="E4">
+        <v>415.1706376040342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2035</v>
+      </c>
+      <c r="B5">
+        <v>178.63382462835557</v>
+      </c>
+      <c r="C5">
+        <v>421.07262275580371</v>
+      </c>
+      <c r="D5">
+        <v>202.15406271210171</v>
+      </c>
+      <c r="E5">
+        <v>444.59286083954987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2040</v>
+      </c>
+      <c r="B6">
+        <v>194.26512837737252</v>
+      </c>
+      <c r="C6">
+        <v>442.65515775541769</v>
+      </c>
+      <c r="D6">
+        <v>228.8354108042094</v>
+      </c>
+      <c r="E6">
+        <v>477.2254401822546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2045</v>
+      </c>
+      <c r="B7">
+        <v>213.15610464009069</v>
+      </c>
+      <c r="C7">
+        <v>467.61453590024161</v>
+      </c>
+      <c r="D7">
+        <v>255.35726611045769</v>
+      </c>
+      <c r="E7">
+        <v>509.81569737060858</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2050</v>
+      </c>
+      <c r="B8">
+        <v>204.01444032563472</v>
+      </c>
+      <c r="C8">
+        <v>454.34869679835845</v>
+      </c>
+      <c r="D8">
+        <v>252.65409354369794</v>
+      </c>
+      <c r="E8">
+        <v>502.98835001642169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C761491-1F84-4914-89BD-A1733E49DA34}">
+  <dimension ref="A1:D169"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>2022</v>
+      </c>
+      <c r="C2">
+        <v>245.91499999999999</v>
+      </c>
+      <c r="D2">
+        <v>178.52799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>2025</v>
+      </c>
+      <c r="C3">
+        <v>261.11099999999999</v>
+      </c>
+      <c r="D3">
+        <v>194.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>2030</v>
+      </c>
+      <c r="C4">
+        <v>269.43700000000001</v>
+      </c>
+      <c r="D4">
+        <v>217.803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>2035</v>
+      </c>
+      <c r="C5">
+        <v>282.44499999999999</v>
+      </c>
+      <c r="D5">
+        <v>242.55699999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>2040</v>
+      </c>
+      <c r="C6">
+        <v>299.46899999999999</v>
+      </c>
+      <c r="D6">
+        <v>270.238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>2045</v>
+      </c>
+      <c r="C7">
+        <v>319.851</v>
+      </c>
+      <c r="D7">
+        <v>297.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>2050</v>
+      </c>
+      <c r="C8">
+        <v>309.94200000000001</v>
+      </c>
+      <c r="D8">
+        <v>294.37299999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>2022</v>
+      </c>
+      <c r="C9">
+        <v>283.77300000000002</v>
+      </c>
+      <c r="D9">
+        <v>216.387</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>2025</v>
+      </c>
+      <c r="C10">
+        <v>299.77199999999999</v>
+      </c>
+      <c r="D10">
+        <v>233.64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>2030</v>
+      </c>
+      <c r="C11">
+        <v>308.91000000000003</v>
+      </c>
+      <c r="D11">
+        <v>257.27699999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2035</v>
+      </c>
+      <c r="C12">
+        <v>322.851</v>
+      </c>
+      <c r="D12">
+        <v>282.96300000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>2040</v>
+      </c>
+      <c r="C13">
+        <v>340.86799999999999</v>
+      </c>
+      <c r="D13">
+        <v>311.637</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2045</v>
+      </c>
+      <c r="C14">
+        <v>362.26100000000002</v>
+      </c>
+      <c r="D14">
+        <v>340.18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2050</v>
+      </c>
+      <c r="C15">
+        <v>351.66399999999999</v>
+      </c>
+      <c r="D15">
+        <v>336.09699999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2022</v>
+      </c>
+      <c r="C16">
+        <v>245.91499999999999</v>
+      </c>
+      <c r="D16">
+        <v>178.52799999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>2025</v>
+      </c>
+      <c r="C17">
+        <v>261.11099999999999</v>
+      </c>
+      <c r="D17">
+        <v>194.98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2030</v>
+      </c>
+      <c r="C18">
+        <v>269.43700000000001</v>
+      </c>
+      <c r="D18">
+        <v>217.803</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>2035</v>
+      </c>
+      <c r="C19">
+        <v>282.44499999999999</v>
+      </c>
+      <c r="D19">
+        <v>242.55699999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>2040</v>
+      </c>
+      <c r="C20">
+        <v>299.46899999999999</v>
+      </c>
+      <c r="D20">
+        <v>270.238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>2045</v>
+      </c>
+      <c r="C21">
+        <v>319.851</v>
+      </c>
+      <c r="D21">
+        <v>297.77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <v>2050</v>
+      </c>
+      <c r="C22">
+        <v>309.94200000000001</v>
+      </c>
+      <c r="D22">
+        <v>294.37299999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>2022</v>
+      </c>
+      <c r="C23">
+        <v>283.77300000000002</v>
+      </c>
+      <c r="D23">
+        <v>216.387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>2025</v>
+      </c>
+      <c r="C24">
+        <v>299.77199999999999</v>
+      </c>
+      <c r="D24">
+        <v>233.64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>2030</v>
+      </c>
+      <c r="C25">
+        <v>308.91000000000003</v>
+      </c>
+      <c r="D25">
+        <v>257.27699999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>2035</v>
+      </c>
+      <c r="C26">
+        <v>322.851</v>
+      </c>
+      <c r="D26">
+        <v>282.96300000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>2040</v>
+      </c>
+      <c r="C27">
+        <v>340.86799999999999</v>
+      </c>
+      <c r="D27">
+        <v>311.637</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>2045</v>
+      </c>
+      <c r="C28">
+        <v>362.26100000000002</v>
+      </c>
+      <c r="D28">
+        <v>340.18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>2050</v>
+      </c>
+      <c r="C29">
+        <v>351.66399999999999</v>
+      </c>
+      <c r="D29">
+        <v>336.09699999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>2022</v>
+      </c>
+      <c r="C30">
+        <v>321.63</v>
+      </c>
+      <c r="D30">
+        <v>254.245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>2025</v>
+      </c>
+      <c r="C31">
+        <v>338.43200000000002</v>
+      </c>
+      <c r="D31">
+        <v>272.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>2030</v>
+      </c>
+      <c r="C32">
+        <v>348.38299999999998</v>
+      </c>
+      <c r="D32">
+        <v>296.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>2035</v>
+      </c>
+      <c r="C33">
+        <v>363.25799999999998</v>
+      </c>
+      <c r="D33">
+        <v>323.37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>2040</v>
+      </c>
+      <c r="C34">
+        <v>382.26600000000002</v>
+      </c>
+      <c r="D34">
+        <v>353.03500000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>2045</v>
+      </c>
+      <c r="C35">
+        <v>404.67099999999999</v>
+      </c>
+      <c r="D35">
+        <v>382.59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>2050</v>
+      </c>
+      <c r="C36">
+        <v>393.38600000000002</v>
+      </c>
+      <c r="D36">
+        <v>377.82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37">
+        <v>2022</v>
+      </c>
+      <c r="C37">
+        <v>283.77300000000002</v>
+      </c>
+      <c r="D37">
+        <v>216.387</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>2025</v>
+      </c>
+      <c r="C38">
+        <v>299.77199999999999</v>
+      </c>
+      <c r="D38">
+        <v>233.64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>2030</v>
+      </c>
+      <c r="C39">
+        <v>308.91000000000003</v>
+      </c>
+      <c r="D39">
+        <v>257.27699999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <v>2035</v>
+      </c>
+      <c r="C40">
+        <v>322.851</v>
+      </c>
+      <c r="D40">
+        <v>282.96300000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>2040</v>
+      </c>
+      <c r="C41">
+        <v>340.86799999999999</v>
+      </c>
+      <c r="D41">
+        <v>311.637</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>2045</v>
+      </c>
+      <c r="C42">
+        <v>362.26100000000002</v>
+      </c>
+      <c r="D42">
+        <v>340.18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43">
+        <v>2050</v>
+      </c>
+      <c r="C43">
+        <v>351.66399999999999</v>
+      </c>
+      <c r="D43">
+        <v>336.09699999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44">
+        <v>2022</v>
+      </c>
+      <c r="C44">
+        <v>321.63</v>
+      </c>
+      <c r="D44">
+        <v>254.245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45">
+        <v>2025</v>
+      </c>
+      <c r="C45">
+        <v>338.43200000000002</v>
+      </c>
+      <c r="D45">
+        <v>272.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46">
+        <v>2030</v>
+      </c>
+      <c r="C46">
+        <v>348.38299999999998</v>
+      </c>
+      <c r="D46">
+        <v>296.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47">
+        <v>2035</v>
+      </c>
+      <c r="C47">
+        <v>363.25799999999998</v>
+      </c>
+      <c r="D47">
+        <v>323.37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <v>2040</v>
+      </c>
+      <c r="C48">
+        <v>382.26600000000002</v>
+      </c>
+      <c r="D48">
+        <v>353.03500000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49">
+        <v>2045</v>
+      </c>
+      <c r="C49">
+        <v>404.67099999999999</v>
+      </c>
+      <c r="D49">
+        <v>382.59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50">
+        <v>2050</v>
+      </c>
+      <c r="C50">
+        <v>393.38600000000002</v>
+      </c>
+      <c r="D50">
+        <v>377.82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51">
+        <v>2022</v>
+      </c>
+      <c r="C51">
+        <v>359.48700000000002</v>
+      </c>
+      <c r="D51">
+        <v>292.10300000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52">
+        <v>2025</v>
+      </c>
+      <c r="C52">
+        <v>377.09300000000002</v>
+      </c>
+      <c r="D52">
+        <v>310.95999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53">
+        <v>2030</v>
+      </c>
+      <c r="C53">
+        <v>387.85599999999999</v>
+      </c>
+      <c r="D53">
+        <v>336.22300000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>2035</v>
+      </c>
+      <c r="C54">
+        <v>403.66399999999999</v>
+      </c>
+      <c r="D54">
+        <v>363.77699999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55">
+        <v>2040</v>
+      </c>
+      <c r="C55">
+        <v>423.66399999999999</v>
+      </c>
+      <c r="D55">
+        <v>394.43299999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56">
+        <v>2045</v>
+      </c>
+      <c r="C56">
+        <v>447.08</v>
+      </c>
+      <c r="D56">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57">
+        <v>2050</v>
+      </c>
+      <c r="C57">
+        <v>435.10899999999998</v>
+      </c>
+      <c r="D57">
+        <v>419.54300000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58">
+        <v>2022</v>
+      </c>
+      <c r="C58">
+        <v>245.91499999999999</v>
+      </c>
+      <c r="D58">
+        <v>178.52799999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59">
+        <v>2025</v>
+      </c>
+      <c r="C59">
+        <v>261.11099999999999</v>
+      </c>
+      <c r="D59">
+        <v>194.98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>2030</v>
+      </c>
+      <c r="C60">
+        <v>269.43700000000001</v>
+      </c>
+      <c r="D60">
+        <v>217.803</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61">
+        <v>2035</v>
+      </c>
+      <c r="C61">
+        <v>282.44499999999999</v>
+      </c>
+      <c r="D61">
+        <v>242.55699999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62">
+        <v>2040</v>
+      </c>
+      <c r="C62">
+        <v>299.46899999999999</v>
+      </c>
+      <c r="D62">
+        <v>270.238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63">
+        <v>2045</v>
+      </c>
+      <c r="C63">
+        <v>319.851</v>
+      </c>
+      <c r="D63">
+        <v>297.77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64">
+        <v>2050</v>
+      </c>
+      <c r="C64">
+        <v>309.94200000000001</v>
+      </c>
+      <c r="D64">
+        <v>294.37299999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65">
+        <v>2022</v>
+      </c>
+      <c r="C65">
+        <v>283.77300000000002</v>
+      </c>
+      <c r="D65">
+        <v>216.387</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66">
+        <v>2025</v>
+      </c>
+      <c r="C66">
+        <v>299.77199999999999</v>
+      </c>
+      <c r="D66">
+        <v>233.64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67">
+        <v>2030</v>
+      </c>
+      <c r="C67">
+        <v>308.91000000000003</v>
+      </c>
+      <c r="D67">
+        <v>257.27699999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68">
+        <v>2035</v>
+      </c>
+      <c r="C68">
+        <v>322.851</v>
+      </c>
+      <c r="D68">
+        <v>282.96300000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69">
+        <v>2040</v>
+      </c>
+      <c r="C69">
+        <v>340.86799999999999</v>
+      </c>
+      <c r="D69">
+        <v>311.637</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70">
+        <v>2045</v>
+      </c>
+      <c r="C70">
+        <v>362.26100000000002</v>
+      </c>
+      <c r="D70">
+        <v>340.18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71">
+        <v>2050</v>
+      </c>
+      <c r="C71">
+        <v>351.66399999999999</v>
+      </c>
+      <c r="D71">
+        <v>336.09699999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72">
+        <v>2022</v>
+      </c>
+      <c r="C72">
+        <v>321.63</v>
+      </c>
+      <c r="D72">
+        <v>254.245</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73">
+        <v>2025</v>
+      </c>
+      <c r="C73">
+        <v>338.43200000000002</v>
+      </c>
+      <c r="D73">
+        <v>272.3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>22</v>
+      </c>
+      <c r="B74">
+        <v>2030</v>
+      </c>
+      <c r="C74">
+        <v>348.38299999999998</v>
+      </c>
+      <c r="D74">
+        <v>296.75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75">
+        <v>2035</v>
+      </c>
+      <c r="C75">
+        <v>363.25799999999998</v>
+      </c>
+      <c r="D75">
+        <v>323.37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76">
+        <v>2040</v>
+      </c>
+      <c r="C76">
+        <v>382.26600000000002</v>
+      </c>
+      <c r="D76">
+        <v>353.03500000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77">
+        <v>2045</v>
+      </c>
+      <c r="C77">
+        <v>404.67099999999999</v>
+      </c>
+      <c r="D77">
+        <v>382.59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78">
+        <v>2050</v>
+      </c>
+      <c r="C78">
+        <v>393.38600000000002</v>
+      </c>
+      <c r="D78">
+        <v>377.82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79">
+        <v>2022</v>
+      </c>
+      <c r="C79">
+        <v>283.77300000000002</v>
+      </c>
+      <c r="D79">
+        <v>216.387</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80">
+        <v>2025</v>
+      </c>
+      <c r="C80">
+        <v>299.77199999999999</v>
+      </c>
+      <c r="D80">
+        <v>233.64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81">
+        <v>2030</v>
+      </c>
+      <c r="C81">
+        <v>308.91000000000003</v>
+      </c>
+      <c r="D81">
+        <v>257.27699999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82">
+        <v>2035</v>
+      </c>
+      <c r="C82">
+        <v>322.851</v>
+      </c>
+      <c r="D82">
+        <v>282.96300000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83">
+        <v>2040</v>
+      </c>
+      <c r="C83">
+        <v>340.86799999999999</v>
+      </c>
+      <c r="D83">
+        <v>311.637</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84">
+        <v>2045</v>
+      </c>
+      <c r="C84">
+        <v>362.26100000000002</v>
+      </c>
+      <c r="D84">
+        <v>340.18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85">
+        <v>2050</v>
+      </c>
+      <c r="C85">
+        <v>351.66399999999999</v>
+      </c>
+      <c r="D85">
+        <v>336.09699999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86">
+        <v>2022</v>
+      </c>
+      <c r="C86">
+        <v>321.63</v>
+      </c>
+      <c r="D86">
+        <v>254.245</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87">
+        <v>2025</v>
+      </c>
+      <c r="C87">
+        <v>338.43200000000002</v>
+      </c>
+      <c r="D87">
+        <v>272.3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88">
+        <v>2030</v>
+      </c>
+      <c r="C88">
+        <v>348.38299999999998</v>
+      </c>
+      <c r="D88">
+        <v>296.75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89">
+        <v>2035</v>
+      </c>
+      <c r="C89">
+        <v>363.25799999999998</v>
+      </c>
+      <c r="D89">
+        <v>323.37</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90">
+        <v>2040</v>
+      </c>
+      <c r="C90">
+        <v>382.26600000000002</v>
+      </c>
+      <c r="D90">
+        <v>353.03500000000003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91">
+        <v>2045</v>
+      </c>
+      <c r="C91">
+        <v>404.67099999999999</v>
+      </c>
+      <c r="D91">
+        <v>382.59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92">
+        <v>2050</v>
+      </c>
+      <c r="C92">
+        <v>393.38600000000002</v>
+      </c>
+      <c r="D92">
+        <v>377.82</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>25</v>
+      </c>
+      <c r="B93">
+        <v>2022</v>
+      </c>
+      <c r="C93">
+        <v>359.48700000000002</v>
+      </c>
+      <c r="D93">
+        <v>292.10300000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>25</v>
+      </c>
+      <c r="B94">
+        <v>2025</v>
+      </c>
+      <c r="C94">
+        <v>377.09300000000002</v>
+      </c>
+      <c r="D94">
+        <v>310.95999999999998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>25</v>
+      </c>
+      <c r="B95">
+        <v>2030</v>
+      </c>
+      <c r="C95">
+        <v>387.85599999999999</v>
+      </c>
+      <c r="D95">
+        <v>336.22300000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>25</v>
+      </c>
+      <c r="B96">
+        <v>2035</v>
+      </c>
+      <c r="C96">
+        <v>403.66399999999999</v>
+      </c>
+      <c r="D96">
+        <v>363.77699999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>25</v>
+      </c>
+      <c r="B97">
+        <v>2040</v>
+      </c>
+      <c r="C97">
+        <v>423.66399999999999</v>
+      </c>
+      <c r="D97">
+        <v>394.43299999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98">
+        <v>2045</v>
+      </c>
+      <c r="C98">
+        <v>447.08</v>
+      </c>
+      <c r="D98">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>25</v>
+      </c>
+      <c r="B99">
+        <v>2050</v>
+      </c>
+      <c r="C99">
+        <v>435.10899999999998</v>
+      </c>
+      <c r="D99">
+        <v>419.54300000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100">
+        <v>2022</v>
+      </c>
+      <c r="C100">
+        <v>321.63</v>
+      </c>
+      <c r="D100">
+        <v>254.245</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101">
+        <v>2025</v>
+      </c>
+      <c r="C101">
+        <v>338.43200000000002</v>
+      </c>
+      <c r="D101">
+        <v>272.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102">
+        <v>2030</v>
+      </c>
+      <c r="C102">
+        <v>348.38299999999998</v>
+      </c>
+      <c r="D102">
+        <v>296.75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103">
+        <v>2035</v>
+      </c>
+      <c r="C103">
+        <v>363.25799999999998</v>
+      </c>
+      <c r="D103">
+        <v>323.37</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104">
+        <v>2040</v>
+      </c>
+      <c r="C104">
+        <v>382.26600000000002</v>
+      </c>
+      <c r="D104">
+        <v>353.03500000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105">
+        <v>2045</v>
+      </c>
+      <c r="C105">
+        <v>404.67099999999999</v>
+      </c>
+      <c r="D105">
+        <v>382.59</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106">
+        <v>2050</v>
+      </c>
+      <c r="C106">
+        <v>393.38600000000002</v>
+      </c>
+      <c r="D106">
+        <v>377.82</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>27</v>
+      </c>
+      <c r="B107">
+        <v>2022</v>
+      </c>
+      <c r="C107">
+        <v>359.48700000000002</v>
+      </c>
+      <c r="D107">
+        <v>292.10300000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>27</v>
+      </c>
+      <c r="B108">
+        <v>2025</v>
+      </c>
+      <c r="C108">
+        <v>377.09300000000002</v>
+      </c>
+      <c r="D108">
+        <v>310.95999999999998</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>27</v>
+      </c>
+      <c r="B109">
+        <v>2030</v>
+      </c>
+      <c r="C109">
+        <v>387.85599999999999</v>
+      </c>
+      <c r="D109">
+        <v>336.22300000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>27</v>
+      </c>
+      <c r="B110">
+        <v>2035</v>
+      </c>
+      <c r="C110">
+        <v>403.66399999999999</v>
+      </c>
+      <c r="D110">
+        <v>363.77699999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>27</v>
+      </c>
+      <c r="B111">
+        <v>2040</v>
+      </c>
+      <c r="C111">
+        <v>423.66399999999999</v>
+      </c>
+      <c r="D111">
+        <v>394.43299999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>27</v>
+      </c>
+      <c r="B112">
+        <v>2045</v>
+      </c>
+      <c r="C112">
+        <v>447.08</v>
+      </c>
+      <c r="D112">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>27</v>
+      </c>
+      <c r="B113">
+        <v>2050</v>
+      </c>
+      <c r="C113">
+        <v>435.10899999999998</v>
+      </c>
+      <c r="D113">
+        <v>419.54300000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>28</v>
+      </c>
+      <c r="B114">
+        <v>2022</v>
+      </c>
+      <c r="C114">
+        <v>283.77300000000002</v>
+      </c>
+      <c r="D114">
+        <v>216.387</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>28</v>
+      </c>
+      <c r="B115">
+        <v>2025</v>
+      </c>
+      <c r="C115">
+        <v>299.77199999999999</v>
+      </c>
+      <c r="D115">
+        <v>233.64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>28</v>
+      </c>
+      <c r="B116">
+        <v>2030</v>
+      </c>
+      <c r="C116">
+        <v>308.91000000000003</v>
+      </c>
+      <c r="D116">
+        <v>257.27699999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>28</v>
+      </c>
+      <c r="B117">
+        <v>2035</v>
+      </c>
+      <c r="C117">
+        <v>322.851</v>
+      </c>
+      <c r="D117">
+        <v>282.96300000000002</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>28</v>
+      </c>
+      <c r="B118">
+        <v>2040</v>
+      </c>
+      <c r="C118">
+        <v>340.86799999999999</v>
+      </c>
+      <c r="D118">
+        <v>311.637</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>28</v>
+      </c>
+      <c r="B119">
+        <v>2045</v>
+      </c>
+      <c r="C119">
+        <v>362.26100000000002</v>
+      </c>
+      <c r="D119">
+        <v>340.18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>28</v>
+      </c>
+      <c r="B120">
+        <v>2050</v>
+      </c>
+      <c r="C120">
+        <v>351.66399999999999</v>
+      </c>
+      <c r="D120">
+        <v>336.09699999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>29</v>
+      </c>
+      <c r="B121">
+        <v>2022</v>
+      </c>
+      <c r="C121">
+        <v>321.63</v>
+      </c>
+      <c r="D121">
+        <v>254.245</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>29</v>
+      </c>
+      <c r="B122">
+        <v>2025</v>
+      </c>
+      <c r="C122">
+        <v>338.43200000000002</v>
+      </c>
+      <c r="D122">
+        <v>272.3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>29</v>
+      </c>
+      <c r="B123">
+        <v>2030</v>
+      </c>
+      <c r="C123">
+        <v>348.38299999999998</v>
+      </c>
+      <c r="D123">
+        <v>296.75</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>29</v>
+      </c>
+      <c r="B124">
+        <v>2035</v>
+      </c>
+      <c r="C124">
+        <v>363.25799999999998</v>
+      </c>
+      <c r="D124">
+        <v>323.37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>29</v>
+      </c>
+      <c r="B125">
+        <v>2040</v>
+      </c>
+      <c r="C125">
+        <v>382.26600000000002</v>
+      </c>
+      <c r="D125">
+        <v>353.03500000000003</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>29</v>
+      </c>
+      <c r="B126">
+        <v>2045</v>
+      </c>
+      <c r="C126">
+        <v>404.67099999999999</v>
+      </c>
+      <c r="D126">
+        <v>382.59</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>29</v>
+      </c>
+      <c r="B127">
+        <v>2050</v>
+      </c>
+      <c r="C127">
+        <v>393.38600000000002</v>
+      </c>
+      <c r="D127">
+        <v>377.82</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>30</v>
+      </c>
+      <c r="B128">
+        <v>2022</v>
+      </c>
+      <c r="C128">
+        <v>359.48700000000002</v>
+      </c>
+      <c r="D128">
+        <v>292.10300000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>30</v>
+      </c>
+      <c r="B129">
+        <v>2025</v>
+      </c>
+      <c r="C129">
+        <v>377.09300000000002</v>
+      </c>
+      <c r="D129">
+        <v>310.95999999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>30</v>
+      </c>
+      <c r="B130">
+        <v>2030</v>
+      </c>
+      <c r="C130">
+        <v>387.85599999999999</v>
+      </c>
+      <c r="D130">
+        <v>336.22300000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>30</v>
+      </c>
+      <c r="B131">
+        <v>2035</v>
+      </c>
+      <c r="C131">
+        <v>403.66399999999999</v>
+      </c>
+      <c r="D131">
+        <v>363.77699999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>30</v>
+      </c>
+      <c r="B132">
+        <v>2040</v>
+      </c>
+      <c r="C132">
+        <v>423.66399999999999</v>
+      </c>
+      <c r="D132">
+        <v>394.43299999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>30</v>
+      </c>
+      <c r="B133">
+        <v>2045</v>
+      </c>
+      <c r="C133">
+        <v>447.08</v>
+      </c>
+      <c r="D133">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>30</v>
+      </c>
+      <c r="B134">
+        <v>2050</v>
+      </c>
+      <c r="C134">
+        <v>435.10899999999998</v>
+      </c>
+      <c r="D134">
+        <v>419.54300000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>31</v>
+      </c>
+      <c r="B135">
+        <v>2022</v>
+      </c>
+      <c r="C135">
+        <v>359.48700000000002</v>
+      </c>
+      <c r="D135">
+        <v>292.10300000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>31</v>
+      </c>
+      <c r="B136">
+        <v>2025</v>
+      </c>
+      <c r="C136">
+        <v>377.09300000000002</v>
+      </c>
+      <c r="D136">
+        <v>310.95999999999998</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>31</v>
+      </c>
+      <c r="B137">
+        <v>2030</v>
+      </c>
+      <c r="C137">
+        <v>387.85599999999999</v>
+      </c>
+      <c r="D137">
+        <v>336.22300000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>31</v>
+      </c>
+      <c r="B138">
+        <v>2035</v>
+      </c>
+      <c r="C138">
+        <v>403.66399999999999</v>
+      </c>
+      <c r="D138">
+        <v>363.77699999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>31</v>
+      </c>
+      <c r="B139">
+        <v>2040</v>
+      </c>
+      <c r="C139">
+        <v>423.66399999999999</v>
+      </c>
+      <c r="D139">
+        <v>394.43299999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>31</v>
+      </c>
+      <c r="B140">
+        <v>2045</v>
+      </c>
+      <c r="C140">
+        <v>447.08</v>
+      </c>
+      <c r="D140">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>31</v>
+      </c>
+      <c r="B141">
+        <v>2050</v>
+      </c>
+      <c r="C141">
+        <v>435.10899999999998</v>
+      </c>
+      <c r="D141">
+        <v>419.54300000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>32</v>
+      </c>
+      <c r="B142">
+        <v>2022</v>
+      </c>
+      <c r="C142">
+        <v>359.48700000000002</v>
+      </c>
+      <c r="D142">
+        <v>292.10300000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>32</v>
+      </c>
+      <c r="B143">
+        <v>2025</v>
+      </c>
+      <c r="C143">
+        <v>377.09300000000002</v>
+      </c>
+      <c r="D143">
+        <v>310.95999999999998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>32</v>
+      </c>
+      <c r="B144">
+        <v>2030</v>
+      </c>
+      <c r="C144">
+        <v>387.85599999999999</v>
+      </c>
+      <c r="D144">
+        <v>336.22300000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>32</v>
+      </c>
+      <c r="B145">
+        <v>2035</v>
+      </c>
+      <c r="C145">
+        <v>403.66399999999999</v>
+      </c>
+      <c r="D145">
+        <v>363.77699999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>32</v>
+      </c>
+      <c r="B146">
+        <v>2040</v>
+      </c>
+      <c r="C146">
+        <v>423.66399999999999</v>
+      </c>
+      <c r="D146">
+        <v>394.43299999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>32</v>
+      </c>
+      <c r="B147">
+        <v>2045</v>
+      </c>
+      <c r="C147">
+        <v>447.08</v>
+      </c>
+      <c r="D147">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>32</v>
+      </c>
+      <c r="B148">
+        <v>2050</v>
+      </c>
+      <c r="C148">
+        <v>435.10899999999998</v>
+      </c>
+      <c r="D148">
+        <v>419.54300000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>33</v>
+      </c>
+      <c r="B149">
+        <v>2022</v>
+      </c>
+      <c r="C149">
+        <v>397.34500000000003</v>
+      </c>
+      <c r="D149">
+        <v>329.96199999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>33</v>
+      </c>
+      <c r="B150">
+        <v>2025</v>
+      </c>
+      <c r="C150">
+        <v>415.75299999999999</v>
+      </c>
+      <c r="D150">
+        <v>349.62</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>33</v>
+      </c>
+      <c r="B151">
+        <v>2030</v>
+      </c>
+      <c r="C151">
+        <v>427.32900000000001</v>
+      </c>
+      <c r="D151">
+        <v>375.697</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>33</v>
+      </c>
+      <c r="B152">
+        <v>2035</v>
+      </c>
+      <c r="C152">
+        <v>444.07</v>
+      </c>
+      <c r="D152">
+        <v>404.18299999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>33</v>
+      </c>
+      <c r="B153">
+        <v>2040</v>
+      </c>
+      <c r="C153">
+        <v>465.06299999999999</v>
+      </c>
+      <c r="D153">
+        <v>435.83199999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>33</v>
+      </c>
+      <c r="B154">
+        <v>2045</v>
+      </c>
+      <c r="C154">
+        <v>489.49</v>
+      </c>
+      <c r="D154">
+        <v>467.41</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>33</v>
+      </c>
+      <c r="B155">
+        <v>2050</v>
+      </c>
+      <c r="C155">
+        <v>476.83100000000002</v>
+      </c>
+      <c r="D155">
+        <v>461.267</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>34</v>
+      </c>
+      <c r="B156">
+        <v>2022</v>
+      </c>
+      <c r="C156">
+        <v>359.48700000000002</v>
+      </c>
+      <c r="D156">
+        <v>292.10300000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>34</v>
+      </c>
+      <c r="B157">
+        <v>2025</v>
+      </c>
+      <c r="C157">
+        <v>377.09300000000002</v>
+      </c>
+      <c r="D157">
+        <v>310.95999999999998</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>34</v>
+      </c>
+      <c r="B158">
+        <v>2030</v>
+      </c>
+      <c r="C158">
+        <v>387.85599999999999</v>
+      </c>
+      <c r="D158">
+        <v>336.22300000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>34</v>
+      </c>
+      <c r="B159">
+        <v>2035</v>
+      </c>
+      <c r="C159">
+        <v>403.66399999999999</v>
+      </c>
+      <c r="D159">
+        <v>363.77699999999999</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>34</v>
+      </c>
+      <c r="B160">
+        <v>2040</v>
+      </c>
+      <c r="C160">
+        <v>423.66399999999999</v>
+      </c>
+      <c r="D160">
+        <v>394.43299999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>34</v>
+      </c>
+      <c r="B161">
+        <v>2045</v>
+      </c>
+      <c r="C161">
+        <v>447.08</v>
+      </c>
+      <c r="D161">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>34</v>
+      </c>
+      <c r="B162">
+        <v>2050</v>
+      </c>
+      <c r="C162">
+        <v>435.10899999999998</v>
+      </c>
+      <c r="D162">
+        <v>419.54300000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>35</v>
+      </c>
+      <c r="B163">
+        <v>2022</v>
+      </c>
+      <c r="C163">
+        <v>397.34500000000003</v>
+      </c>
+      <c r="D163">
+        <v>329.96199999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>35</v>
+      </c>
+      <c r="B164">
+        <v>2025</v>
+      </c>
+      <c r="C164">
+        <v>415.75299999999999</v>
+      </c>
+      <c r="D164">
+        <v>349.62</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>35</v>
+      </c>
+      <c r="B165">
+        <v>2030</v>
+      </c>
+      <c r="C165">
+        <v>427.32900000000001</v>
+      </c>
+      <c r="D165">
+        <v>375.697</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>35</v>
+      </c>
+      <c r="B166">
+        <v>2035</v>
+      </c>
+      <c r="C166">
+        <v>444.07</v>
+      </c>
+      <c r="D166">
+        <v>404.18299999999999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>35</v>
+      </c>
+      <c r="B167">
+        <v>2040</v>
+      </c>
+      <c r="C167">
+        <v>465.06299999999999</v>
+      </c>
+      <c r="D167">
+        <v>435.83199999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>35</v>
+      </c>
+      <c r="B168">
+        <v>2045</v>
+      </c>
+      <c r="C168">
+        <v>489.49</v>
+      </c>
+      <c r="D168">
+        <v>467.41</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>35</v>
+      </c>
+      <c r="B169">
+        <v>2050</v>
+      </c>
+      <c r="C169">
+        <v>476.83100000000002</v>
+      </c>
+      <c r="D169">
+        <v>461.267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493886F6-E811-4F57-AFA1-5E6483BC75C2}">
   <dimension ref="A1:Q178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.125" customWidth="1"/>
-    <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="15.875" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="6.125" customWidth="1"/>
-    <col min="10" max="10" width="49.375" customWidth="1"/>
-    <col min="11" max="17" width="10.5" customWidth="1"/>
+    <col min="7" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" customWidth="1"/>
+    <col min="10" max="10" width="49.42578125" customWidth="1"/>
+    <col min="11" max="17" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>2022</v>
       </c>
@@ -635,7 +3346,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +3396,7 @@
         <v>204.01444032563472</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -735,7 +3446,7 @@
         <v>454.34869679835845</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -785,7 +3496,7 @@
         <v>252.65409354369794</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -835,7 +3546,7 @@
         <v>502.98835001642169</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>40</v>
       </c>
@@ -843,7 +3554,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -857,7 +3568,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -871,7 +3582,7 @@
         <v>178.52799999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -888,7 +3599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -902,7 +3613,7 @@
         <v>217.803</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -916,7 +3627,7 @@
         <v>242.55699999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -930,7 +3641,7 @@
         <v>270.238</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -944,7 +3655,7 @@
         <v>297.77</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -958,7 +3669,7 @@
         <v>294.37299999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -972,7 +3683,7 @@
         <v>216.387</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -986,7 +3697,7 @@
         <v>233.64</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1000,7 +3711,7 @@
         <v>257.27699999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1014,7 +3725,7 @@
         <v>282.96300000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +3739,7 @@
         <v>311.637</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1042,7 +3753,7 @@
         <v>340.18</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1056,7 +3767,7 @@
         <v>336.09699999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1070,7 +3781,7 @@
         <v>178.52799999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1084,7 +3795,7 @@
         <v>194.98</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1098,7 +3809,7 @@
         <v>217.803</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +3823,7 @@
         <v>242.55699999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1126,7 +3837,7 @@
         <v>270.238</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1140,7 +3851,7 @@
         <v>297.77</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1154,7 +3865,7 @@
         <v>294.37299999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1168,7 +3879,7 @@
         <v>216.387</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1182,7 +3893,7 @@
         <v>233.64</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1196,7 +3907,7 @@
         <v>257.27699999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1210,7 +3921,7 @@
         <v>282.96300000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1224,7 +3935,7 @@
         <v>311.637</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1238,7 +3949,7 @@
         <v>340.18</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -1252,7 +3963,7 @@
         <v>336.09699999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1266,7 +3977,7 @@
         <v>254.245</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1280,7 +3991,7 @@
         <v>272.3</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1294,7 +4005,7 @@
         <v>296.75</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -1308,7 +4019,7 @@
         <v>323.37</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1322,7 +4033,7 @@
         <v>353.03500000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -1336,7 +4047,7 @@
         <v>382.59</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -1350,7 +4061,7 @@
         <v>377.82</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1364,7 +4075,7 @@
         <v>216.387</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1378,7 +4089,7 @@
         <v>233.64</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +4103,7 @@
         <v>257.27699999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +4117,7 @@
         <v>282.96300000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +4131,7 @@
         <v>311.637</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -1434,7 +4145,7 @@
         <v>340.18</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1448,7 +4159,7 @@
         <v>336.09699999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1462,7 +4173,7 @@
         <v>254.245</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -1476,7 +4187,7 @@
         <v>272.3</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -1490,7 +4201,7 @@
         <v>296.75</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -1504,7 +4215,7 @@
         <v>323.37</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -1518,7 +4229,7 @@
         <v>353.03500000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -1532,7 +4243,7 @@
         <v>382.59</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -1546,7 +4257,7 @@
         <v>377.82</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1560,7 +4271,7 @@
         <v>292.10300000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -1574,7 +4285,7 @@
         <v>310.95999999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -1588,7 +4299,7 @@
         <v>336.22300000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -1602,7 +4313,7 @@
         <v>363.77699999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -1616,7 +4327,7 @@
         <v>394.43299999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -1630,7 +4341,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -1644,7 +4355,7 @@
         <v>419.54300000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +4369,7 @@
         <v>178.52799999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -1672,7 +4383,7 @@
         <v>194.98</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>20</v>
       </c>
@@ -1686,7 +4397,7 @@
         <v>217.803</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>20</v>
       </c>
@@ -1700,7 +4411,7 @@
         <v>242.55699999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>20</v>
       </c>
@@ -1714,7 +4425,7 @@
         <v>270.238</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>20</v>
       </c>
@@ -1728,7 +4439,7 @@
         <v>297.77</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>20</v>
       </c>
@@ -1742,7 +4453,7 @@
         <v>294.37299999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>21</v>
       </c>
@@ -1756,7 +4467,7 @@
         <v>216.387</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>21</v>
       </c>
@@ -1770,7 +4481,7 @@
         <v>233.64</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>21</v>
       </c>
@@ -1784,7 +4495,7 @@
         <v>257.27699999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1798,7 +4509,7 @@
         <v>282.96300000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>21</v>
       </c>
@@ -1812,7 +4523,7 @@
         <v>311.637</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>21</v>
       </c>
@@ -1826,7 +4537,7 @@
         <v>340.18</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>21</v>
       </c>
@@ -1840,7 +4551,7 @@
         <v>336.09699999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -1854,7 +4565,7 @@
         <v>254.245</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -1868,7 +4579,7 @@
         <v>272.3</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>22</v>
       </c>
@@ -1882,7 +4593,7 @@
         <v>296.75</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>22</v>
       </c>
@@ -1896,7 +4607,7 @@
         <v>323.37</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>22</v>
       </c>
@@ -1910,7 +4621,7 @@
         <v>353.03500000000003</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -1924,7 +4635,7 @@
         <v>382.59</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -1938,7 +4649,7 @@
         <v>377.82</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>23</v>
       </c>
@@ -1952,7 +4663,7 @@
         <v>216.387</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>23</v>
       </c>
@@ -1966,7 +4677,7 @@
         <v>233.64</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>23</v>
       </c>
@@ -1980,7 +4691,7 @@
         <v>257.27699999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>23</v>
       </c>
@@ -1994,7 +4705,7 @@
         <v>282.96300000000002</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +4719,7 @@
         <v>311.637</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>23</v>
       </c>
@@ -2022,7 +4733,7 @@
         <v>340.18</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>23</v>
       </c>
@@ -2036,7 +4747,7 @@
         <v>336.09699999999998</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -2050,7 +4761,7 @@
         <v>254.245</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -2064,7 +4775,7 @@
         <v>272.3</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -2078,7 +4789,7 @@
         <v>296.75</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>24</v>
       </c>
@@ -2092,7 +4803,7 @@
         <v>323.37</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>24</v>
       </c>
@@ -2106,7 +4817,7 @@
         <v>353.03500000000003</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>24</v>
       </c>
@@ -2120,7 +4831,7 @@
         <v>382.59</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>24</v>
       </c>
@@ -2134,7 +4845,7 @@
         <v>377.82</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>25</v>
       </c>
@@ -2148,7 +4859,7 @@
         <v>292.10300000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>25</v>
       </c>
@@ -2162,7 +4873,7 @@
         <v>310.95999999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>25</v>
       </c>
@@ -2176,7 +4887,7 @@
         <v>336.22300000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>25</v>
       </c>
@@ -2190,7 +4901,7 @@
         <v>363.77699999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>25</v>
       </c>
@@ -2204,7 +4915,7 @@
         <v>394.43299999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>25</v>
       </c>
@@ -2218,7 +4929,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>25</v>
       </c>
@@ -2232,7 +4943,7 @@
         <v>419.54300000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>26</v>
       </c>
@@ -2246,7 +4957,7 @@
         <v>254.245</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>26</v>
       </c>
@@ -2260,7 +4971,7 @@
         <v>272.3</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>26</v>
       </c>
@@ -2274,7 +4985,7 @@
         <v>296.75</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>26</v>
       </c>
@@ -2288,7 +4999,7 @@
         <v>323.37</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>26</v>
       </c>
@@ -2302,7 +5013,7 @@
         <v>353.03500000000003</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>26</v>
       </c>
@@ -2316,7 +5027,7 @@
         <v>382.59</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>26</v>
       </c>
@@ -2330,7 +5041,7 @@
         <v>377.82</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>27</v>
       </c>
@@ -2344,7 +5055,7 @@
         <v>292.10300000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>27</v>
       </c>
@@ -2358,7 +5069,7 @@
         <v>310.95999999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>27</v>
       </c>
@@ -2372,7 +5083,7 @@
         <v>336.22300000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>27</v>
       </c>
@@ -2386,7 +5097,7 @@
         <v>363.77699999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>27</v>
       </c>
@@ -2400,7 +5111,7 @@
         <v>394.43299999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>27</v>
       </c>
@@ -2414,7 +5125,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>27</v>
       </c>
@@ -2428,7 +5139,7 @@
         <v>419.54300000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>28</v>
       </c>
@@ -2442,7 +5153,7 @@
         <v>216.387</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>28</v>
       </c>
@@ -2456,7 +5167,7 @@
         <v>233.64</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>28</v>
       </c>
@@ -2470,7 +5181,7 @@
         <v>257.27699999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>28</v>
       </c>
@@ -2484,7 +5195,7 @@
         <v>282.96300000000002</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>28</v>
       </c>
@@ -2498,7 +5209,7 @@
         <v>311.637</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>28</v>
       </c>
@@ -2512,7 +5223,7 @@
         <v>340.18</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>28</v>
       </c>
@@ -2526,7 +5237,7 @@
         <v>336.09699999999998</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>29</v>
       </c>
@@ -2540,7 +5251,7 @@
         <v>254.245</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>29</v>
       </c>
@@ -2554,7 +5265,7 @@
         <v>272.3</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>29</v>
       </c>
@@ -2568,7 +5279,7 @@
         <v>296.75</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>29</v>
       </c>
@@ -2582,7 +5293,7 @@
         <v>323.37</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>29</v>
       </c>
@@ -2596,7 +5307,7 @@
         <v>353.03500000000003</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>29</v>
       </c>
@@ -2610,7 +5321,7 @@
         <v>382.59</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>29</v>
       </c>
@@ -2624,7 +5335,7 @@
         <v>377.82</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>30</v>
       </c>
@@ -2638,7 +5349,7 @@
         <v>292.10300000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>30</v>
       </c>
@@ -2652,7 +5363,7 @@
         <v>310.95999999999998</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>30</v>
       </c>
@@ -2666,7 +5377,7 @@
         <v>336.22300000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>30</v>
       </c>
@@ -2680,7 +5391,7 @@
         <v>363.77699999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>30</v>
       </c>
@@ -2694,7 +5405,7 @@
         <v>394.43299999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>30</v>
       </c>
@@ -2708,7 +5419,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>30</v>
       </c>
@@ -2722,7 +5433,7 @@
         <v>419.54300000000001</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>31</v>
       </c>
@@ -2736,7 +5447,7 @@
         <v>292.10300000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>31</v>
       </c>
@@ -2750,7 +5461,7 @@
         <v>310.95999999999998</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>31</v>
       </c>
@@ -2764,7 +5475,7 @@
         <v>336.22300000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>31</v>
       </c>
@@ -2778,7 +5489,7 @@
         <v>363.77699999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>31</v>
       </c>
@@ -2792,7 +5503,7 @@
         <v>394.43299999999999</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>31</v>
       </c>
@@ -2806,7 +5517,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>31</v>
       </c>
@@ -2820,7 +5531,7 @@
         <v>419.54300000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>32</v>
       </c>
@@ -2834,7 +5545,7 @@
         <v>292.10300000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>32</v>
       </c>
@@ -2848,7 +5559,7 @@
         <v>310.95999999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>32</v>
       </c>
@@ -2862,7 +5573,7 @@
         <v>336.22300000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>32</v>
       </c>
@@ -2876,7 +5587,7 @@
         <v>363.77699999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>32</v>
       </c>
@@ -2890,7 +5601,7 @@
         <v>394.43299999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>32</v>
       </c>
@@ -2904,7 +5615,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>32</v>
       </c>
@@ -2918,7 +5629,7 @@
         <v>419.54300000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>33</v>
       </c>
@@ -2932,7 +5643,7 @@
         <v>329.96199999999999</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>33</v>
       </c>
@@ -2946,7 +5657,7 @@
         <v>349.62</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>33</v>
       </c>
@@ -2960,7 +5671,7 @@
         <v>375.697</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>33</v>
       </c>
@@ -2974,7 +5685,7 @@
         <v>404.18299999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>33</v>
       </c>
@@ -2988,7 +5699,7 @@
         <v>435.83199999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>33</v>
       </c>
@@ -3002,7 +5713,7 @@
         <v>467.41</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>33</v>
       </c>
@@ -3016,7 +5727,7 @@
         <v>461.267</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>34</v>
       </c>
@@ -3030,7 +5741,7 @@
         <v>292.10300000000001</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>34</v>
       </c>
@@ -3044,7 +5755,7 @@
         <v>310.95999999999998</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>34</v>
       </c>
@@ -3058,7 +5769,7 @@
         <v>336.22300000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>34</v>
       </c>
@@ -3072,7 +5783,7 @@
         <v>363.77699999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>34</v>
       </c>
@@ -3086,7 +5797,7 @@
         <v>394.43299999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>34</v>
       </c>
@@ -3100,7 +5811,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>34</v>
       </c>
@@ -3114,7 +5825,7 @@
         <v>419.54300000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>35</v>
       </c>
@@ -3128,7 +5839,7 @@
         <v>329.96199999999999</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>35</v>
       </c>
@@ -3142,7 +5853,7 @@
         <v>349.62</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>35</v>
       </c>
@@ -3156,7 +5867,7 @@
         <v>375.697</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>35</v>
       </c>
@@ -3170,7 +5881,7 @@
         <v>404.18299999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>35</v>
       </c>
@@ -3184,7 +5895,7 @@
         <v>435.83199999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>35</v>
       </c>
@@ -3198,7 +5909,7 @@
         <v>467.41</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>35</v>
       </c>

</xml_diff>